<commit_message>
login & signup page
</commit_message>
<xml_diff>
--- a/cypress/class2testCase.xlsx
+++ b/cypress/class2testCase.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6741f279e29cc654/桌面/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\work\cy\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="232" documentId="11_F25DC773A252ABDACC10488CF15F72F65BDE58EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E766B688-D039-4974-BB25-013296A663B8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07E3E034-20DD-4453-A90A-B5739F047507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4875" yWindow="5295" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3555" yWindow="4755" windowWidth="27105" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="73">
   <si>
     <t>Test case ID</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -71,14 +71,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>TC_HOME_H_04</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>TC_HOME_H_05</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Verify the navigation bar is visible</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -95,10 +87,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>navigation bar should have 5 links</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>navigation bar have 5 links</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -107,14 +95,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>links in the navigation is visible</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Click the link to switch pages</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>links is visible</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -125,9 +105,6 @@
   <si>
     <t>2. click link</t>
     <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Functionality of the navigation bar</t>
   </si>
   <si>
     <t>Functionality of the navigation bar</t>
@@ -188,10 +165,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Click the logo switch to homepages</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>logo is visible</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -216,22 +189,10 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>navigation bar should always visible</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>navigation bar is visible</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>navigation bar should be visible</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>TC_HOME_H_06</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>navigation bar should always on top of the page</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -273,6 +234,138 @@
   </si>
   <si>
     <t>header visible all time</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>navigation bar should have 5 visible links</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Click the link to switch pages &amp;&amp;Click the logo switch to homepages</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC_LOGIN_01</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Login form is visible </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">form has 3 roles </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>visit ‘cms-lyart.vercel.app/login’</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>form for 3 roles student, teacher, manager</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC_LOGIN_02</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">login form format </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>email format</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>aaa</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>input aaa on email input</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>clear the email input</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">is not a valid email" shows </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>email' is required" shows</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>have 3 roles and student is defult</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>hit shows</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC_LOGIN_03</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>password format</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>same with 02</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>same above</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC_LOGIN_04</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>verify login</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>login with student, teacher, manager</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>input email and password and click sign in button</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>student, teacher,manager, (111111)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>should success login and to the dashboard page</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC_LOGIN_05</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sign up link</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>click sign up link should bring to sign up page</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>click 'sign up' link</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>should on the sign up page</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>on the sign up page</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -359,37 +452,46 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -672,301 +774,417 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10:H11"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.25" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.75" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.75" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.375" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19" style="5" customWidth="1"/>
-    <col min="9" max="9" width="17.625" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9" style="5"/>
+    <col min="1" max="1" width="14.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.25" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.75" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.75" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.375" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19" style="3" customWidth="1"/>
+    <col min="9" max="9" width="17.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="4"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="4"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" s="9"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="9"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="8" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="5" t="s">
+      <c r="H6" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="I6" s="9"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="9"/>
+    </row>
+    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="F8" s="10"/>
+      <c r="G8" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I8" s="9"/>
+    </row>
+    <row r="9" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="11"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="9"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="11"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="11"/>
+      <c r="G10" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="11"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="11"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="I2" s="8"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="8"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H4" s="3" t="s">
+      <c r="G12" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="I4" s="9"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="9"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="H6" s="10" t="s">
+      <c r="H12" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="I6" s="9"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="9"/>
-    </row>
-    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+      <c r="B13" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="H8" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="I8" s="9"/>
-    </row>
-    <row r="9" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" s="1" t="s">
+      <c r="E13" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="9"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="6"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="5" customFormat="1" ht="57" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>72</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="28">
+  <mergeCells count="32">
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="C8:C11"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C4:C7"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G8:G9"/>
     <mergeCell ref="G10:G11"/>
     <mergeCell ref="H8:H9"/>
     <mergeCell ref="H10:H11"/>
     <mergeCell ref="I8:I9"/>
     <mergeCell ref="I10:I11"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H4:H5"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
course format & case
</commit_message>
<xml_diff>
--- a/cypress/class2testCase.xlsx
+++ b/cypress/class2testCase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\work\cy\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07E3E034-20DD-4453-A90A-B5739F047507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F00779E-3D7A-4982-8CE9-EB9113C0DCF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3555" yWindow="4755" windowWidth="27105" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="84">
   <si>
     <t>Test case ID</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -366,6 +366,49 @@
   </si>
   <si>
     <t>on the sign up page</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC_COURSE_01</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC_COURSE_02</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>add course</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>edit course</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>use manager to add a course</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>use manager to edit a course</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>able to visit the website, able to login with manager</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1.visit website 2. click sign in link 3. click manager 4. enter email and password 5. click sign in button 6. click course 7. click add course 8. enter all detial 9. click create course 10. enter schedule detial 11. click button </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{ "createdAt": "2022-08-18 04:14:20","updatedAt": "2022-08-18 04:14:20","id": 1706,"cover": "http://lorempixel.com/800/600/technics/","detail": "e2e abc example need have 100 word x xxxxx xxxxx xxxxx xxxx xxxx xxxx xxxx xxxx xxxx xxxx xxxx xxxx.103","duration": 30,"durationUnit": 5,"maxStudents": 10,"name": "aaa","price": 5000,"uid": "c5e80093-a777-4ef1-96a6-799c691665f0","star": 0,"startTime": "2022-08-19 08:00:00","status": 0,"scheduleId": 2146,"teacherId": 77,"type": [ { "id": 1,"name": "C" } ],"teacherName": "Fanny Haag" }</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Successfully Create Course! Page shows up</t>
+  </si>
+  <si>
+    <t>Successfully Create Course! Page shows up</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -452,7 +495,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -470,28 +513,34 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -774,10 +823,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -787,7 +836,7 @@
     <col min="3" max="3" width="32.75" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.75" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="32.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17" style="3" customWidth="1"/>
     <col min="7" max="7" width="35.375" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19" style="3" customWidth="1"/>
     <col min="9" max="9" width="17.625" style="3" bestFit="1" customWidth="1"/>
@@ -824,16 +873,16 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="3" t="s">
@@ -851,10 +900,10 @@
       <c r="I2" s="4"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
       <c r="E3" s="3" t="s">
         <v>13</v>
       </c>
@@ -870,13 +919,13 @@
       <c r="I3" s="4"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="11" t="s">
         <v>41</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -885,135 +934,135 @@
       <c r="E4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="I4" s="9"/>
+      <c r="I4" s="12"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="12"/>
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="11"/>
       <c r="D5" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="9"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="12"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="12"/>
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="11"/>
       <c r="D6" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H6" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="I6" s="9"/>
+      <c r="I6" s="12"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="12"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="11"/>
       <c r="D7" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="9"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="12"/>
     </row>
     <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10" t="s">
+      <c r="F8" s="14"/>
+      <c r="G8" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="H8" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="I8" s="9"/>
+      <c r="I8" s="12"/>
     </row>
     <row r="9" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="11"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
       <c r="E9" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="9"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="12"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="11"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="12" t="s">
+      <c r="A10" s="9"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="11" t="s">
         <v>31</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="11"/>
-      <c r="G10" s="6" t="s">
+      <c r="F10" s="9"/>
+      <c r="G10" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="11"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="12"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="11"/>
       <c r="E11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="11"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
@@ -1039,16 +1088,16 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E13" s="3" t="s">
@@ -1065,14 +1114,14 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="11"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
       <c r="E14" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G14" s="13" t="s">
+      <c r="G14" s="8" t="s">
         <v>54</v>
       </c>
       <c r="H14" s="3" t="s">
@@ -1151,13 +1200,58 @@
         <v>72</v>
       </c>
     </row>
+    <row r="18" spans="1:8" ht="195" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A19" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="F4:F5"/>
     <mergeCell ref="H4:H5"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A4:A7"/>
@@ -1172,19 +1266,14 @@
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="F10:F11"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="F4:F5"/>
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="G8:G9"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="G4:G5"/>
     <mergeCell ref="G10:G11"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="I10:I11"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>